<commit_message>
Replace black screen with motion sickness video and update test mode in video generation script
- Swap 5-second black screen with 'mareo.mp4' in video sequence generation
- Set test mode to True by default in generate_videos function
- Add suprablock_count to confidence luminance instructions sequence
- Update order matrix files for subject 12 in results and output directories
</commit_message>
<xml_diff>
--- a/results/sub-12/order_matrix_12_A_block1_VR.xlsx
+++ b/results/sub-12/order_matrix_12_A_block1_VR.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,11 +593,11 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>./instructions_videos/block_3_text.mp4</t>
+          <t>./instructions_videos/block_4_text.mp4</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -632,7 +632,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -642,16 +642,16 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>direct</t>
+          <t>inverse</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/13.mp4</t>
+          <t>../stimuli/exp_videos/VR/2.mp4</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -687,11 +687,11 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
+          <t>./instructions_videos/post_stimulus_self_report.mp4</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -701,7 +701,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>instruction_post_stimulus_verbal_report</t>
+          <t>post_stimulus_self_report</t>
         </is>
       </c>
     </row>
@@ -727,11 +727,11 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>./videos_fixation/countdown_bar.mp4</t>
+          <t>./instructions_videos/mareo.mp4</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -741,7 +741,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>verbal_report</t>
+          <t>motion_sickness</t>
         </is>
       </c>
     </row>
@@ -767,11 +767,11 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>./instructions_videos/confidence_verbal_report_text.mp4</t>
+          <t>./instructions_videos/block_4_text_reminder.mp4</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -781,7 +781,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>confidence_verbal_report</t>
+          <t>audio_instruction</t>
         </is>
       </c>
     </row>
@@ -801,17 +801,31 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>valence</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>./black_screen_5_sec.mp4</t>
+          <t>../stimuli/exp_videos/VR/12.mp4</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -821,7 +835,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>black_screen_5_seconds</t>
+          <t>video</t>
         </is>
       </c>
     </row>
@@ -847,11 +861,11 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>./instructions_videos/block_3_text_reminder.mp4</t>
+          <t>./instructions_videos/post_stimulus_self_report.mp4</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -861,7 +875,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>audio_instruction</t>
+          <t>post_stimulus_self_report</t>
         </is>
       </c>
     </row>
@@ -881,31 +895,17 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>2</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>valence</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>direct</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/6.mp4</t>
+          <t>./instructions_videos/mareo.mp4</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
@@ -915,7 +915,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>video</t>
+          <t>motion_sickness</t>
         </is>
       </c>
     </row>
@@ -941,11 +941,11 @@
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
+          <t>./instructions_videos/block_4_text_reminder.mp4</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
@@ -955,7 +955,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>instruction_post_stimulus_verbal_report</t>
+          <t>audio_instruction</t>
         </is>
       </c>
     </row>
@@ -975,17 +975,31 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="D13" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>valence</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>./videos_fixation/countdown_bar.mp4</t>
+          <t>../stimuli/exp_videos/VR/3.mp4</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J13" t="n">
         <v>0</v>
@@ -995,7 +1009,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>verbal_report</t>
+          <t>video</t>
         </is>
       </c>
     </row>
@@ -1021,11 +1035,11 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>./instructions_videos/confidence_verbal_report_text.mp4</t>
+          <t>./instructions_videos/post_stimulus_self_report.mp4</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -1035,7 +1049,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>confidence_verbal_report</t>
+          <t>post_stimulus_self_report</t>
         </is>
       </c>
     </row>
@@ -1061,11 +1075,11 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>./black_screen_5_sec.mp4</t>
+          <t>./instructions_videos/mareo.mp4</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
@@ -1075,7 +1089,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>black_screen_5_seconds</t>
+          <t>motion_sickness</t>
         </is>
       </c>
     </row>
@@ -1101,12 +1115,10 @@
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
-          <t>./instructions_videos/block_3_text_reminder.mp4</t>
-        </is>
-      </c>
-      <c r="I16" t="n">
-        <v>3</v>
-      </c>
+          <t>./instructions_videos/luminance_instructions_inverse.mp4</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="n">
         <v>0</v>
       </c>
@@ -1115,7 +1127,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>audio_instruction</t>
+          <t>luminance_instructions</t>
         </is>
       </c>
     </row>
@@ -1136,31 +1148,25 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>valence</t>
+          <t>luminance</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>direct</t>
+          <t>inverse</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/14.mp4</t>
-        </is>
-      </c>
-      <c r="I17" t="n">
-        <v>3</v>
-      </c>
+          <t>../stimuli/exp_videos/VR/green_intensity_video_12.mp4</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
       <c r="J17" t="n">
         <v>0</v>
       </c>
@@ -1169,7 +1175,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>video</t>
+          <t>luminance</t>
         </is>
       </c>
     </row>
@@ -1195,12 +1201,10 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
-        </is>
-      </c>
-      <c r="I18" t="n">
-        <v>3</v>
-      </c>
+          <t>./instructions_videos/confidence_luminance_practice_instructions_text.mp4</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
       <c r="J18" t="n">
         <v>0</v>
       </c>
@@ -1209,7 +1213,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>instruction_post_stimulus_verbal_report</t>
+          <t>confidence_luminance_instructions</t>
         </is>
       </c>
     </row>
@@ -1235,21 +1239,21 @@
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>./videos_fixation/countdown_bar.mp4</t>
+          <t>./instructions_videos/block_1_text.mp4</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" t="n">
         <v>1</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>verbal_report</t>
+          <t>audio_instruction</t>
         </is>
       </c>
     </row>
@@ -1269,27 +1273,41 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+      <c r="D20" t="n">
+        <v>5</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>arousal</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>./instructions_videos/confidence_verbal_report_text.mp4</t>
+          <t>../stimuli/exp_videos/VR/4.mp4</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" t="n">
         <v>1</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>confidence_verbal_report</t>
+          <t>video</t>
         </is>
       </c>
     </row>
@@ -1315,21 +1333,21 @@
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>./black_screen_5_sec.mp4</t>
+          <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" t="n">
         <v>1</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>black_screen_5_seconds</t>
+          <t>instruction_post_stimulus_verbal_report</t>
         </is>
       </c>
     </row>
@@ -1355,19 +1373,21 @@
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>./instructions_videos/luminance_instructions_direct.mp4</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr"/>
+          <t>./videos_fixation/countdown_bar.mp4</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" t="n">
         <v>1</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>luminance_instructions</t>
+          <t>verbal_report</t>
         </is>
       </c>
     </row>
@@ -1387,35 +1407,27 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D23" t="n">
-        <v>4</v>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>luminance</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>direct</t>
-        </is>
-      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/green_intensity_video_9.mp4</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr"/>
+          <t>./instructions_videos/confidence_verbal_report_text.mp4</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>1</v>
+      </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" t="n">
         <v>1</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>luminance</t>
+          <t>confidence_verbal_report</t>
         </is>
       </c>
     </row>
@@ -1441,11 +1453,11 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>./instructions_videos/block_2_text.mp4</t>
+          <t>./instructions_videos/mareo.mp4</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J24" t="n">
         <v>1</v>
@@ -1455,7 +1467,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>audio_instruction</t>
+          <t>motion_sickness</t>
         </is>
       </c>
     </row>
@@ -1475,31 +1487,17 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D25" t="n">
-        <v>5</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>arousal</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">inverse </t>
-        </is>
-      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/1.mp4</t>
+          <t>./instructions_videos/block_1_text_reminder.mp4</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25" t="n">
         <v>1</v>
@@ -1509,7 +1507,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>video</t>
+          <t>audio_instruction</t>
         </is>
       </c>
     </row>
@@ -1529,17 +1527,31 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+      <c r="D26" t="n">
+        <v>6</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>arousal</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>./instructions_videos/post_stimulus_self_report.mp4</t>
+          <t>../stimuli/exp_videos/VR/9.mp4</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J26" t="n">
         <v>1</v>
@@ -1549,7 +1561,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>post_stimulus_self_report</t>
+          <t>video</t>
         </is>
       </c>
     </row>
@@ -1575,11 +1587,11 @@
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>./black_screen_5_sec.mp4</t>
+          <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J27" t="n">
         <v>1</v>
@@ -1589,7 +1601,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>black_screen_5_seconds</t>
+          <t>instruction_post_stimulus_verbal_report</t>
         </is>
       </c>
     </row>
@@ -1615,11 +1627,11 @@
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>./instructions_videos/block_2_text_reminder.mp4</t>
+          <t>./videos_fixation/countdown_bar.mp4</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J28" t="n">
         <v>1</v>
@@ -1629,7 +1641,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>audio_instruction</t>
+          <t>verbal_report</t>
         </is>
       </c>
     </row>
@@ -1649,31 +1661,17 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D29" t="n">
-        <v>6</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>arousal</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>inverse</t>
-        </is>
-      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/10.mp4</t>
+          <t>./instructions_videos/confidence_verbal_report_text.mp4</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J29" t="n">
         <v>1</v>
@@ -1683,7 +1681,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>video</t>
+          <t>confidence_verbal_report</t>
         </is>
       </c>
     </row>
@@ -1709,11 +1707,11 @@
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>./instructions_videos/post_stimulus_self_report.mp4</t>
+          <t>./instructions_videos/mareo.mp4</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J30" t="n">
         <v>1</v>
@@ -1723,7 +1721,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>post_stimulus_self_report</t>
+          <t>motion_sickness</t>
         </is>
       </c>
     </row>
@@ -1749,11 +1747,11 @@
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>./black_screen_5_sec.mp4</t>
+          <t>./instructions_videos/block_1_text_reminder.mp4</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J31" t="n">
         <v>1</v>
@@ -1763,7 +1761,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>black_screen_5_seconds</t>
+          <t>audio_instruction</t>
         </is>
       </c>
     </row>
@@ -1783,17 +1781,31 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
+      <c r="D32" t="n">
+        <v>7</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>arousal</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
+      </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>./instructions_videos/block_2_text_reminder.mp4</t>
+          <t>../stimuli/exp_videos/VR/7.mp4</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J32" t="n">
         <v>1</v>
@@ -1803,7 +1815,7 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>audio_instruction</t>
+          <t>video</t>
         </is>
       </c>
     </row>
@@ -1823,31 +1835,17 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D33" t="n">
-        <v>7</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>arousal</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>inverse</t>
-        </is>
-      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/5.mp4</t>
+          <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J33" t="n">
         <v>1</v>
@@ -1857,7 +1855,7 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>video</t>
+          <t>instruction_post_stimulus_verbal_report</t>
         </is>
       </c>
     </row>
@@ -1883,11 +1881,11 @@
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>./instructions_videos/post_stimulus_self_report.mp4</t>
+          <t>./videos_fixation/countdown_bar.mp4</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J34" t="n">
         <v>1</v>
@@ -1897,7 +1895,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>post_stimulus_self_report</t>
+          <t>verbal_report</t>
         </is>
       </c>
     </row>
@@ -1923,11 +1921,11 @@
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>./black_screen_5_sec.mp4</t>
+          <t>./instructions_videos/confidence_verbal_report_text.mp4</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J35" t="n">
         <v>1</v>
@@ -1937,7 +1935,7 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>black_screen_5_seconds</t>
+          <t>confidence_verbal_report</t>
         </is>
       </c>
     </row>
@@ -1963,11 +1961,11 @@
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>./instructions_videos/block_2_text_reminder.mp4</t>
+          <t>./instructions_videos/mareo.mp4</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J36" t="n">
         <v>1</v>
@@ -1977,7 +1975,7 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>audio_instruction</t>
+          <t>motion_sickness</t>
         </is>
       </c>
     </row>
@@ -1997,31 +1995,17 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D37" t="n">
-        <v>8</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>arousal</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>inverse</t>
-        </is>
-      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/11.mp4</t>
+          <t>./instructions_videos/block_1_text_reminder.mp4</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J37" t="n">
         <v>1</v>
@@ -2031,7 +2015,7 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>video</t>
+          <t>audio_instruction</t>
         </is>
       </c>
     </row>
@@ -2051,17 +2035,31 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
+      <c r="D38" t="n">
+        <v>8</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>arousal</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
+      </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>./instructions_videos/post_stimulus_self_report.mp4</t>
+          <t>../stimuli/exp_videos/VR/8.mp4</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J38" t="n">
         <v>1</v>
@@ -2071,7 +2069,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>post_stimulus_self_report</t>
+          <t>video</t>
         </is>
       </c>
     </row>
@@ -2097,11 +2095,11 @@
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>./black_screen_5_sec.mp4</t>
+          <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J39" t="n">
         <v>1</v>
@@ -2111,7 +2109,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>black_screen_5_seconds</t>
+          <t>instruction_post_stimulus_verbal_report</t>
         </is>
       </c>
     </row>
@@ -2137,10 +2135,12 @@
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>./instructions_videos/luminance_instructions_direct.mp4</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr"/>
+          <t>./videos_fixation/countdown_bar.mp4</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>1</v>
+      </c>
       <c r="J40" t="n">
         <v>1</v>
       </c>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>luminance_instructions</t>
+          <t>verbal_report</t>
         </is>
       </c>
     </row>
@@ -2169,26 +2169,18 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D41" t="n">
-        <v>9</v>
-      </c>
+      <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>luminance</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">inverse </t>
-        </is>
-      </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/green_intensity_video_7.mp4</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr"/>
+          <t>./instructions_videos/confidence_verbal_report_text.mp4</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>1</v>
+      </c>
       <c r="J41" t="n">
         <v>1</v>
       </c>
@@ -2197,7 +2189,7 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>luminance</t>
+          <t>confidence_verbal_report</t>
         </is>
       </c>
     </row>
@@ -2223,17 +2215,181 @@
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
+          <t>./instructions_videos/mareo.mp4</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>1</v>
+      </c>
+      <c r="J42" t="n">
+        <v>1</v>
+      </c>
+      <c r="K42" t="n">
+        <v>1</v>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>motion_sickness</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>A_block1</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>VR</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>./instructions_videos/luminance_instructions_direct.mp4</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="n">
+        <v>1</v>
+      </c>
+      <c r="K43" t="n">
+        <v>1</v>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>luminance_instructions</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>A_block1</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>VR</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>9</v>
+      </c>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>luminance</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>../stimuli/exp_videos/VR/green_intensity_video_3.mp4</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="n">
+        <v>1</v>
+      </c>
+      <c r="K44" t="n">
+        <v>1</v>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>luminance</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>A_block1</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>VR</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>./instructions_videos/confidence_luminance_practice_instructions_text.mp4</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="n">
+        <v>1</v>
+      </c>
+      <c r="K45" t="n">
+        <v>1</v>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>confidence_luminance_instructions</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>A_block1</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>VR</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr">
+        <is>
           <t>./instructions_videos/rest_suprablock_text.mp4</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr"/>
-      <c r="J42" t="n">
-        <v>1</v>
-      </c>
-      <c r="K42" t="n">
-        <v>1</v>
-      </c>
-      <c r="L42" t="inlineStr">
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="n">
+        <v>1</v>
+      </c>
+      <c r="K46" t="n">
+        <v>1</v>
+      </c>
+      <c r="L46" t="inlineStr">
         <is>
           <t>rest_suprablock</t>
         </is>

</xml_diff>